<commit_message>
todo generado para julio 2022
</commit_message>
<xml_diff>
--- a/txt generated files/planillas que se necesitan para generar el txt/Benef_UGL.xlsx
+++ b/txt generated files/planillas que se necesitan para generar el txt/Benef_UGL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\OneDrive\Documentos\txtgenerator\txtgenerator\txt generated files\planillas que se necesitan para generar el txt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EBE479A-234F-4638-9B69-65F0BC33811F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4499D6C-D494-474C-BE6D-5F91A7485FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,26 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>nroAfiliado</t>
   </si>
   <si>
     <t>ugl</t>
   </si>
-  <si>
-    <t>09595992810000</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,9 +65,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B245"/>
+  <dimension ref="A1:B247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A245"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,1955 +397,1971 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>15584685550000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>15035746200100</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>15023912910700</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>15057792390500</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>46590310310300</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>11595020050200</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>15040832450500</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>15076855530300</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>15027046450100</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>15528063040005</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>15030778850700</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>14091900940100</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>15031832480300</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>15017202370100</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>15018084590100</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>15006088660400</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>15097318920100</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>15060235740100</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>9092909500300</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>15098559440500</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>15051655100600</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>15069072230800</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>15010091340000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>46501931990900</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>15036796620700</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>15068119460600</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>15028393790100</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>15001052930000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>15040437110100</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>14090932480200</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>2009226280700</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>11593957100600</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>15037416330400</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>15017590970500</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>40507307050200</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>15034520610600</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>11095379790816</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>15591456680400</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>15059316650800</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>15083289150300</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>40507819150200</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>15060785890100</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>15041889460200</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>46590287290500</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>15598573230900</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>15022477800800</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>15027517780100</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>15511000450400</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>15022618100200</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>15049671820100</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>15083943090000</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>9095199060800</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>15538289400516</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>15049831850500</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>15026946730500</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>14005974260600</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>15035475360600</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>15055817710900</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>9005349230700</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>15042335970700</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>10561961530100</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>15582319441400</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>4010284340800</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>15053494560100</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>15013921260700</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>15081799660100</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>15014028790400</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>15078069070300</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>11095379790800</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>15088215870600</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>15023658490100</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>15084721410100</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>14594248470500</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>15060169930800</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>15533496881100</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>11521381000800</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>15044314040800</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>15585363400900</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>15026259520101</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>15031777950100</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>15086219020800</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>15031498540800</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>5520139230300</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>15010623600400</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>15589978940400</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>15052714680100</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>15031410580900</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>2009417000500</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>15083495650000</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>15027155420100</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>15039626710400</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>15040008750900</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>14594615540600</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>15013453130500</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>15019497100600</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>15070662660700</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>10054868000100</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>14004417110100</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>15020990410700</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>15028035090100</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="A102" s="2">
         <v>9531742130400</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103" s="2">
         <v>15012920140300</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+      <c r="A104" s="2">
         <v>15010781910200</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="A105" s="2">
         <v>14001014470200</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+      <c r="A106" s="2">
         <v>15084936000900</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="A107" s="2">
         <v>15549604100300</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="A108" s="2">
         <v>40507429460600</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="A109" s="2">
         <v>15067318930901</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="A110" s="2">
         <v>15013178380600</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="A111" s="2">
         <v>15046549800200</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+      <c r="A112" s="2">
         <v>15082908560800</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="A113" s="2">
         <v>15044572750016</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+      <c r="A114" s="2">
         <v>1008672310000</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115" s="2">
         <v>15011805800200</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+      <c r="A116" s="2">
         <v>15047916080300</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+      <c r="A117" s="2">
         <v>7632826021200</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+      <c r="A118" s="2">
         <v>15084721410100</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+      <c r="A119" s="2">
         <v>15029072670700</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+      <c r="A120" s="2">
         <v>15073766820000</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+      <c r="A121" s="2">
         <v>15048257980500</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+      <c r="A122" s="2">
         <v>15036598130400</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+      <c r="A123" s="2">
         <v>15065104740400</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+      <c r="A124" s="2">
         <v>15008884170900</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+      <c r="A125" s="2">
         <v>40506918490100</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+      <c r="A126" s="2">
         <v>15007492390000</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+      <c r="A127" s="2">
         <v>15022463560800</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+      <c r="A128" s="2">
         <v>15018716560400</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+      <c r="A129" s="2">
         <v>15510439930500</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+      <c r="A130" s="2">
         <v>15030346200600</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+      <c r="A131" s="2">
         <v>15017883630200</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
+      <c r="A132" s="2">
         <v>15065802360300</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+      <c r="A133" s="2">
         <v>15018193080800</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
+      <c r="A134" s="2">
         <v>15037830590300</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
+      <c r="A135" s="2">
         <v>15083088820800</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
+      <c r="A136" s="2">
         <v>15040385370100</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+      <c r="A137" s="2">
         <v>15018050240300</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+      <c r="A138" s="2">
         <v>15038524570100</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+      <c r="A139" s="2">
         <v>15039239310500</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+      <c r="A140" s="2">
         <v>1501851801700</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
+      <c r="A141" s="2">
         <v>15059518920600</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+      <c r="A142" s="2">
         <v>3532747570600</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+      <c r="A143" s="2">
         <v>15098004200300</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+      <c r="A144" s="2">
         <v>15082134130100</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+      <c r="A145" s="2">
         <v>15089134250000</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+      <c r="A146" s="2">
         <v>15018340030200</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+      <c r="A147" s="2">
         <v>9560666960100</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
+      <c r="A148" s="2">
         <v>15052977230500</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
+      <c r="A149" s="2">
         <v>13515110740300</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+      <c r="A150" s="2">
         <v>15029059500500</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+      <c r="A151" s="2">
         <v>15072857090000</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+      <c r="A152" s="2">
         <v>15086735630500</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
+      <c r="A153" s="2">
         <v>9596420620200</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
+      <c r="A154" s="2">
         <v>15085791300816</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+      <c r="A155" s="2">
         <v>15060440750900</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
+      <c r="A156" s="2">
         <v>15071396370700</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+      <c r="A157" s="2">
         <v>15039776680400</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+      <c r="A158" s="2">
         <v>15077497990900</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+      <c r="A159" s="2">
         <v>15051963380200</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
+      <c r="A160" s="2">
         <v>15073772090716</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+      <c r="A161" s="2">
         <v>15075575690700</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+      <c r="A162" s="2">
         <v>9096278380700</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+      <c r="A163" s="2">
         <v>15052063990716</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+      <c r="A164" s="2">
         <v>15021130970901</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+      <c r="A165" s="2">
         <v>15049007600100</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+      <c r="A166" s="2">
         <v>11092100780700</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
+      <c r="A167" s="2">
         <v>46590165350900</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B168">
+      <c r="A168" s="2">
+        <v>9595992810000</v>
+      </c>
+      <c r="B168" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+      <c r="A169" s="2">
         <v>15043863830700</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
+      <c r="A170" s="2">
         <v>15049588570800</v>
       </c>
-      <c r="B170">
+      <c r="B170" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+      <c r="A171" s="2">
         <v>13055083660300</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
+      <c r="A172" s="2">
         <v>9561309640100</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+      <c r="A173" s="2">
         <v>15011522410900</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+      <c r="A174" s="2">
         <v>15587865340700</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+      <c r="A175" s="2">
         <v>15524478320000</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
+      <c r="A176" s="2">
         <v>14592894090100</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
+      <c r="A177" s="2">
         <v>15021130970900</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+      <c r="A178" s="2">
         <v>15043511480101</v>
       </c>
-      <c r="B178">
+      <c r="B178" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
+      <c r="A179" s="2">
         <v>15032839340300</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+      <c r="A180" s="2">
         <v>40507102310900</v>
       </c>
-      <c r="B180">
+      <c r="B180" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+      <c r="A181" s="2">
         <v>15583838450200</v>
       </c>
-      <c r="B181">
+      <c r="B181" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+      <c r="A182" s="2">
         <v>15031640950900</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+      <c r="A183" s="2">
         <v>46590083030101</v>
       </c>
-      <c r="B183">
+      <c r="B183" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+      <c r="A184" s="2">
         <v>15087703520000</v>
       </c>
-      <c r="B184">
+      <c r="B184" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
+      <c r="A185" s="2">
         <v>15024666350100</v>
       </c>
-      <c r="B185">
+      <c r="B185" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
+      <c r="A186" s="2">
         <v>15087565370601</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+      <c r="A187" s="2">
         <v>15029288650600</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+      <c r="A188" s="2">
         <v>15013586900400</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+      <c r="A189" s="2">
         <v>15010954070800</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
+      <c r="A190" s="2">
         <v>15086139760700</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+      <c r="A191" s="2">
         <v>40507063710300</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+      <c r="A192" s="2">
         <v>15033740760600</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
+      <c r="A193" s="2">
         <v>15081884470300</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+      <c r="A194" s="2">
         <v>15016129830700</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
+      <c r="A195" s="2">
         <v>14003202900400</v>
       </c>
-      <c r="B195">
+      <c r="B195" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
+      <c r="A196" s="2">
         <v>15502464020800</v>
       </c>
-      <c r="B196">
+      <c r="B196" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
+      <c r="A197" s="2">
         <v>15001540450900</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+      <c r="A198" s="2">
         <v>15018745920100</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+      <c r="A199" s="2">
         <v>13053892670100</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
+      <c r="A200" s="2">
         <v>15016481250600</v>
       </c>
-      <c r="B200">
+      <c r="B200" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
+      <c r="A201" s="2">
         <v>15058469550200</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
+      <c r="A202" s="2">
         <v>15055636130800</v>
       </c>
-      <c r="B202">
+      <c r="B202" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
+      <c r="A203" s="2">
         <v>15075790980800</v>
       </c>
-      <c r="B203">
+      <c r="B203" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
+      <c r="A204" s="2">
         <v>15083495650000</v>
       </c>
-      <c r="B204">
+      <c r="B204" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
+      <c r="A205" s="2">
         <v>15040008750900</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
+      <c r="A206" s="2">
         <v>15080294300200</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
+      <c r="A207" s="2">
         <v>3010174510700</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
+      <c r="A208" s="2">
         <v>15052456860000</v>
       </c>
-      <c r="B208">
+      <c r="B208" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
+      <c r="A209" s="2">
         <v>15046897230300</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
+      <c r="A210" s="2">
         <v>15005891920800</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+      <c r="A211" s="2">
         <v>15514107690200</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
+      <c r="A212" s="2">
         <v>15083342130300</v>
       </c>
-      <c r="B212">
+      <c r="B212" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
+      <c r="A213" s="2">
         <v>15061489920800</v>
       </c>
-      <c r="B213">
+      <c r="B213" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="1">
+      <c r="A214" s="2">
         <v>15084722670100</v>
       </c>
-      <c r="B214">
+      <c r="B214" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+      <c r="A215" s="2">
         <v>15017703940700</v>
       </c>
-      <c r="B215">
+      <c r="B215" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="A216" s="2">
         <v>5590242650100</v>
       </c>
-      <c r="B216">
+      <c r="B216" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
+      <c r="A217" s="2">
         <v>1003916420100</v>
       </c>
-      <c r="B217">
+      <c r="B217" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
+      <c r="A218" s="2">
         <v>6530625961000</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+      <c r="A219" s="2">
         <v>15562070450700</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="1">
+      <c r="A220" s="2">
         <v>15059439300100</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="1">
+      <c r="A221" s="2">
         <v>15044688780600</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="1">
+      <c r="A222" s="2">
         <v>15069947690600</v>
       </c>
-      <c r="B222">
+      <c r="B222" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
+      <c r="A223" s="2">
         <v>15024407010100</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+      <c r="A224" s="2">
         <v>15066195970400</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
+      <c r="A225" s="2">
         <v>11095773750100</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="1">
+      <c r="A226" s="2">
         <v>15593192870100</v>
       </c>
-      <c r="B226">
+      <c r="B226" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
+      <c r="A227" s="2">
         <v>15020240430000</v>
       </c>
-      <c r="B227">
+      <c r="B227" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+      <c r="A228" s="2">
         <v>15063518060000</v>
       </c>
-      <c r="B228">
+      <c r="B228" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
+      <c r="A229" s="2">
         <v>15052066080000</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
+      <c r="A230" s="2">
         <v>15026439930800</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="1">
+      <c r="A231" s="2">
         <v>11594490290100</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
+      <c r="A232" s="2">
         <v>15028095550301</v>
       </c>
-      <c r="B232">
+      <c r="B232" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
+      <c r="A233" s="2">
         <v>13050565610600</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
+      <c r="A234" s="2">
         <v>15086309000600</v>
       </c>
-      <c r="B234">
+      <c r="B234" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="1">
+      <c r="A235" s="2">
         <v>9595992810000</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="1">
+      <c r="A236" s="2">
         <v>11521862820200</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
+      <c r="A237" s="2">
         <v>15063582620400</v>
       </c>
-      <c r="B237">
+      <c r="B237" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="1">
+      <c r="A238" s="2">
         <v>15052546570500</v>
       </c>
-      <c r="B238">
+      <c r="B238" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
+      <c r="A239" s="2">
         <v>10053979200700</v>
       </c>
-      <c r="B239">
+      <c r="B239" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
+      <c r="A240" s="2">
         <v>15069308400100</v>
       </c>
-      <c r="B240">
+      <c r="B240" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
+      <c r="A241" s="2">
         <v>15035201650400</v>
       </c>
-      <c r="B241">
+      <c r="B241" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="1">
+      <c r="A242" s="2">
         <v>15006029040400</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="1">
+      <c r="A243" s="2">
         <v>15010057240700</v>
       </c>
-      <c r="B243">
+      <c r="B243" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
+      <c r="A244" s="2">
         <v>15089250550100</v>
       </c>
-      <c r="B244">
+      <c r="B244" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
+      <c r="A245" s="2">
         <v>15535894290100</v>
       </c>
-      <c r="B245">
-        <v>31</v>
+      <c r="B245" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>15003177820000</v>
+      </c>
+      <c r="B246" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>15043777240100</v>
+      </c>
+      <c r="B247" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios varios generando hasta agosto incluyendo generado de junio y julio de nuevo
</commit_message>
<xml_diff>
--- a/txt generated files/planillas que se necesitan para generar el txt/Benef_UGL.xlsx
+++ b/txt generated files/planillas que se necesitan para generar el txt/Benef_UGL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\OneDrive\Documentos\txtgenerator\txtgenerator\txt generated files\planillas que se necesitan para generar el txt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA650BEF-2EEC-45B1-8A28-138BF8DD924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B80D754-397B-4D06-804E-6AFF35B9477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C248"/>
+  <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158:XFD158"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,178 +401,178 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>14594615540600</v>
+        <v>15584685550000</v>
       </c>
       <c r="B2" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>15027155420100</v>
+        <v>15035746200100</v>
       </c>
       <c r="B3" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>15055090080800</v>
+        <v>15023912910700</v>
       </c>
       <c r="B4" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>15043777240100</v>
+        <v>15057792390500</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>15003177820000</v>
+        <v>46590310310300</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>15535894290100</v>
+        <v>11595020050200</v>
       </c>
       <c r="B7" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>15089250550100</v>
+        <v>15040832450500</v>
       </c>
       <c r="B8" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>15010057240700</v>
+        <v>15076855530300</v>
       </c>
       <c r="B9" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>15006029040400</v>
+        <v>15027046450100</v>
       </c>
       <c r="B10" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>15035201650400</v>
+        <v>15528063040005</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>15069308400100</v>
+        <v>15030778850700</v>
       </c>
       <c r="B12" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>10053979200700</v>
+        <v>14091900940100</v>
       </c>
       <c r="B13" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>15052546570500</v>
+        <v>15031832480300</v>
       </c>
       <c r="B14" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>15063582620400</v>
+        <v>15017202370100</v>
       </c>
       <c r="B15" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>11521862820200</v>
+        <v>15018084590100</v>
       </c>
       <c r="B16" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>9595992810000</v>
+        <v>15006088660400</v>
       </c>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>15086309000600</v>
+        <v>15097318920100</v>
       </c>
       <c r="B18" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>13050565610600</v>
+        <v>15060235740100</v>
       </c>
       <c r="B19" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>15028095550301</v>
+        <v>9092909500300</v>
       </c>
       <c r="B20" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>11594490290100</v>
+        <v>15098559440500</v>
       </c>
       <c r="B21" s="1">
         <v>10</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>15026439930800</v>
+        <v>15051655100600</v>
       </c>
       <c r="B22" s="1">
         <v>10</v>
@@ -590,43 +590,43 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>15052066080000</v>
+        <v>15069072230800</v>
       </c>
       <c r="B23" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>15063518060000</v>
+        <v>15010091340000</v>
       </c>
       <c r="B24" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>15020240430000</v>
+        <v>46501931990900</v>
       </c>
       <c r="B25" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>15593192870100</v>
+        <v>15036796620700</v>
       </c>
       <c r="B26" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>11095773750100</v>
+        <v>15068119460600</v>
       </c>
       <c r="B27" s="1">
         <v>10</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>15066195970400</v>
+        <v>15028393790100</v>
       </c>
       <c r="B28" s="1">
         <v>10</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>15024407010100</v>
+        <v>15001052930000</v>
       </c>
       <c r="B29" s="1">
         <v>10</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>15069947690600</v>
+        <v>15040437110100</v>
       </c>
       <c r="B30" s="1">
         <v>10</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>15044688780600</v>
+        <v>14090932480200</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>15059439300100</v>
+        <v>2009226280700</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>15562070450700</v>
+        <v>11593957100600</v>
       </c>
       <c r="B33" s="1">
         <v>10</v>
@@ -689,34 +689,34 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>6530625961000</v>
+        <v>15037416330400</v>
       </c>
       <c r="B34" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>1003916420100</v>
+        <v>15017590970500</v>
       </c>
       <c r="B35" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>5590242650100</v>
+        <v>40507307050200</v>
       </c>
       <c r="B36" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>15017703940700</v>
+        <v>15034520610600</v>
       </c>
       <c r="B37" s="1">
         <v>10</v>
@@ -725,25 +725,25 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>15084722670100</v>
+        <v>11095379790816</v>
       </c>
       <c r="B38" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>15061489920800</v>
+        <v>15591456680400</v>
       </c>
       <c r="B39" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>15083342130300</v>
+        <v>15059316650800</v>
       </c>
       <c r="B40" s="1">
         <v>10</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>15514107690200</v>
+        <v>15083289150300</v>
       </c>
       <c r="B41" s="1">
         <v>10</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>15005891920800</v>
+        <v>40507819150200</v>
       </c>
       <c r="B42" s="1">
         <v>10</v>
@@ -770,619 +770,619 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>15046897230300</v>
+        <v>15060785890100</v>
       </c>
       <c r="B43" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>15052456860000</v>
+        <v>15041889460200</v>
       </c>
       <c r="B44" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>3010174510700</v>
+        <v>46590287290500</v>
       </c>
       <c r="B45" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>15080294300200</v>
+        <v>15598573230900</v>
       </c>
       <c r="B46" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>15040008750900</v>
+        <v>15022477800800</v>
       </c>
       <c r="B47" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>15083495650000</v>
+        <v>15027517780100</v>
       </c>
       <c r="B48" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>15075790980800</v>
+        <v>15511000450400</v>
       </c>
       <c r="B49" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>15055636130800</v>
+        <v>15022618100200</v>
       </c>
       <c r="B50" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>15058469550200</v>
+        <v>15049671820100</v>
       </c>
       <c r="B51" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>15016481250600</v>
+        <v>15083943090000</v>
       </c>
       <c r="B52" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C52" s="3"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>13053892670100</v>
+        <v>9095199060800</v>
       </c>
       <c r="B53" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>15018745920100</v>
+        <v>15538289400516</v>
       </c>
       <c r="B54" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>15001540450900</v>
+        <v>15049831850500</v>
       </c>
       <c r="B55" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>15502464020800</v>
+        <v>15026946730500</v>
       </c>
       <c r="B56" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>14003202900400</v>
+        <v>14005974260600</v>
       </c>
       <c r="B57" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>15016129830700</v>
+        <v>15035475360600</v>
       </c>
       <c r="B58" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>15081884470300</v>
+        <v>15055817710900</v>
       </c>
       <c r="B59" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C59" s="3"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>15033740760600</v>
+        <v>9005349230700</v>
       </c>
       <c r="B60" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>40507063710300</v>
+        <v>15042335970700</v>
       </c>
       <c r="B61" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>15086139760700</v>
+        <v>10561961530100</v>
       </c>
       <c r="B62" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>15010954070800</v>
+        <v>15582319441400</v>
       </c>
       <c r="B63" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>15013586900400</v>
+        <v>4010284340800</v>
       </c>
       <c r="B64" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>15029288650600</v>
+        <v>15053494560100</v>
       </c>
       <c r="B65" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C65" s="3"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>15087565370601</v>
+        <v>15013921260700</v>
       </c>
       <c r="B66" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>15024666350100</v>
+        <v>15081799660100</v>
       </c>
       <c r="B67" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>15087703520000</v>
+        <v>15014028790400</v>
       </c>
       <c r="B68" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>46590083030101</v>
+        <v>15078069070300</v>
       </c>
       <c r="B69" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>15031640950900</v>
+        <v>11095379790800</v>
       </c>
       <c r="B70" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>15583838450200</v>
+        <v>15088215870600</v>
       </c>
       <c r="B71" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C71" s="3"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>40507102310900</v>
+        <v>15023658490100</v>
       </c>
       <c r="B72" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C72" s="3"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>15032839340300</v>
+        <v>15084721410100</v>
       </c>
       <c r="B73" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>15043511480101</v>
+        <v>14594248470500</v>
       </c>
       <c r="B74" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C74" s="3"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>15021130970900</v>
+        <v>15060169930800</v>
       </c>
       <c r="B75" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C75" s="3"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>14592894090100</v>
+        <v>15533496881100</v>
       </c>
       <c r="B76" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>15524478320000</v>
+        <v>11521381000800</v>
       </c>
       <c r="B77" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>15587865340700</v>
+        <v>15044314040800</v>
       </c>
       <c r="B78" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C78" s="3"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>15011522410900</v>
+        <v>15585363400900</v>
       </c>
       <c r="B79" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>9561309640100</v>
+        <v>15026259520101</v>
       </c>
       <c r="B80" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C80" s="3"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>13055083660300</v>
+        <v>15031777950100</v>
       </c>
       <c r="B81" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>15049588570800</v>
+        <v>15086219020800</v>
       </c>
       <c r="B82" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C82" s="3"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>15043863830700</v>
+        <v>15031498540800</v>
       </c>
       <c r="B83" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>9595992810000</v>
+        <v>5520139230300</v>
       </c>
       <c r="B84" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>46590165350900</v>
+        <v>15010623600400</v>
       </c>
       <c r="B85" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>11092100780700</v>
+        <v>15589978940400</v>
       </c>
       <c r="B86" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>15049007600100</v>
+        <v>15052714680100</v>
       </c>
       <c r="B87" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>15021130970901</v>
+        <v>15031410580900</v>
       </c>
       <c r="B88" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>15052063990716</v>
+        <v>2009417000500</v>
       </c>
       <c r="B89" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>9096278380700</v>
+        <v>15083495650000</v>
       </c>
       <c r="B90" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>15075575690700</v>
+        <v>15027155420100</v>
       </c>
       <c r="B91" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C91" s="3"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>15073772090716</v>
+        <v>15039626710400</v>
       </c>
       <c r="B92" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>15051963380200</v>
+        <v>15040008750900</v>
       </c>
       <c r="B93" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C93" s="3"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>15077497990900</v>
+        <v>14594615540600</v>
       </c>
       <c r="B94" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C94" s="3"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>15039776680400</v>
+        <v>15013453130500</v>
       </c>
       <c r="B95" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C95" s="3"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>15071396370700</v>
+        <v>15019497100600</v>
       </c>
       <c r="B96" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C96" s="3"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>15060440750900</v>
+        <v>15070662660700</v>
       </c>
       <c r="B97" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C97" s="3"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>15085791300816</v>
+        <v>10054868000100</v>
       </c>
       <c r="B98" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C98" s="3"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>9596420620200</v>
+        <v>14004417110100</v>
       </c>
       <c r="B99" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C99" s="3"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>15086735630500</v>
+        <v>15020990410700</v>
       </c>
       <c r="B100" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C100" s="3"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>15072857090000</v>
+        <v>15028035090100</v>
       </c>
       <c r="B101" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>15029059500500</v>
+        <v>9531742130400</v>
       </c>
       <c r="B102" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C102" s="3"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>13515110740300</v>
+        <v>15012920140300</v>
       </c>
       <c r="B103" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C103" s="3"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>15052977230500</v>
+        <v>15010781910200</v>
       </c>
       <c r="B104" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C104" s="3"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>9560666960100</v>
+        <v>14001014470200</v>
       </c>
       <c r="B105" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C105" s="3"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>15018340030200</v>
+        <v>15084936000900</v>
       </c>
       <c r="B106" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C106" s="3"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>15089134250000</v>
+        <v>15549604100300</v>
       </c>
       <c r="B107" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C107" s="3"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>15082134130100</v>
+        <v>40507429460600</v>
       </c>
       <c r="B108" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C108" s="3"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>15098004200300</v>
+        <v>15067318930901</v>
       </c>
       <c r="B109" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>3532747570600</v>
+        <v>15013178380600</v>
       </c>
       <c r="B110" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C110" s="3"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>15059518920600</v>
+        <v>15046549800200</v>
       </c>
       <c r="B111" s="1">
         <v>6</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>1501851801700</v>
+        <v>15082908560800</v>
       </c>
       <c r="B112" s="1">
         <v>6</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>15039239310500</v>
+        <v>15044572750016</v>
       </c>
       <c r="B113" s="1">
         <v>6</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>15038524570100</v>
+        <v>1008672310000</v>
       </c>
       <c r="B114" s="1">
         <v>6</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>15018050240300</v>
+        <v>15011805800200</v>
       </c>
       <c r="B115" s="1">
         <v>6</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>15040385370100</v>
+        <v>15047916080300</v>
       </c>
       <c r="B116" s="1">
         <v>6</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>15083088820800</v>
+        <v>7632826021200</v>
       </c>
       <c r="B117" s="1">
         <v>6</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>15037830590300</v>
+        <v>15084721410100</v>
       </c>
       <c r="B118" s="1">
         <v>6</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>15018193080800</v>
+        <v>15029072670700</v>
       </c>
       <c r="B119" s="1">
         <v>6</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>15065802360300</v>
+        <v>15073766820000</v>
       </c>
       <c r="B120" s="1">
         <v>6</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>15017883630200</v>
+        <v>15048257980500</v>
       </c>
       <c r="B121" s="1">
         <v>6</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>15030346200600</v>
+        <v>15036598130400</v>
       </c>
       <c r="B122" s="1">
         <v>6</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>15510439930500</v>
+        <v>15065104740400</v>
       </c>
       <c r="B123" s="1">
         <v>6</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>15018716560400</v>
+        <v>15008884170900</v>
       </c>
       <c r="B124" s="1">
         <v>6</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>15022463560800</v>
+        <v>40506918490100</v>
       </c>
       <c r="B125" s="1">
         <v>6</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>40506918490100</v>
+        <v>15022463560800</v>
       </c>
       <c r="B127" s="1">
         <v>6</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>15008884170900</v>
+        <v>15018716560400</v>
       </c>
       <c r="B128" s="1">
         <v>6</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>15065104740400</v>
+        <v>15510439930500</v>
       </c>
       <c r="B129" s="1">
         <v>6</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>15036598130400</v>
+        <v>15030346200600</v>
       </c>
       <c r="B130" s="1">
         <v>6</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>15048257980500</v>
+        <v>15017883630200</v>
       </c>
       <c r="B131" s="1">
         <v>6</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>15073766820000</v>
+        <v>15065802360300</v>
       </c>
       <c r="B132" s="1">
         <v>6</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>15029072670700</v>
+        <v>15018193080800</v>
       </c>
       <c r="B133" s="1">
         <v>6</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>15084721410100</v>
+        <v>15037830590300</v>
       </c>
       <c r="B134" s="1">
         <v>6</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>7632826021200</v>
+        <v>15083088820800</v>
       </c>
       <c r="B135" s="1">
         <v>6</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>15047916080300</v>
+        <v>15040385370100</v>
       </c>
       <c r="B136" s="1">
         <v>6</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>15011805800200</v>
+        <v>15018050240300</v>
       </c>
       <c r="B137" s="1">
         <v>6</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>1008672310000</v>
+        <v>15038524570100</v>
       </c>
       <c r="B138" s="1">
         <v>6</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>15044572750016</v>
+        <v>15039239310500</v>
       </c>
       <c r="B139" s="1">
         <v>6</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>15082908560800</v>
+        <v>1501851801700</v>
       </c>
       <c r="B140" s="1">
         <v>6</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>15046549800200</v>
+        <v>15059518920600</v>
       </c>
       <c r="B141" s="1">
         <v>6</v>
@@ -1661,619 +1661,619 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>15013178380600</v>
+        <v>3532747570600</v>
       </c>
       <c r="B142" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C142" s="3"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>15067318930901</v>
+        <v>15098004200300</v>
       </c>
       <c r="B143" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C143" s="3"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>40507429460600</v>
+        <v>15082134130100</v>
       </c>
       <c r="B144" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C144" s="3"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>15549604100300</v>
+        <v>15089134250000</v>
       </c>
       <c r="B145" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>15084936000900</v>
+        <v>15018340030200</v>
       </c>
       <c r="B146" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C146" s="3"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>14001014470200</v>
+        <v>9560666960100</v>
       </c>
       <c r="B147" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C147" s="3"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>15010781910200</v>
+        <v>15052977230500</v>
       </c>
       <c r="B148" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C148" s="3"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>15012920140300</v>
+        <v>13515110740300</v>
       </c>
       <c r="B149" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>9531742130400</v>
+        <v>15029059500500</v>
       </c>
       <c r="B150" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C150" s="3"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>15028035090100</v>
+        <v>15072857090000</v>
       </c>
       <c r="B151" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C151" s="3"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>15020990410700</v>
+        <v>15086735630500</v>
       </c>
       <c r="B152" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C152" s="3"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>14004417110100</v>
+        <v>9596420620200</v>
       </c>
       <c r="B153" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>10054868000100</v>
+        <v>15085791300816</v>
       </c>
       <c r="B154" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C154" s="3"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>15070662660700</v>
+        <v>15060440750900</v>
       </c>
       <c r="B155" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C155" s="3"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>15019497100600</v>
+        <v>15071396370700</v>
       </c>
       <c r="B156" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C156" s="3"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>15013453130500</v>
+        <v>15039776680400</v>
       </c>
       <c r="B157" s="1">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>15040008750900</v>
+        <v>15077497990900</v>
       </c>
       <c r="B158" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C158" s="3"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>15039626710400</v>
+        <v>15051963380200</v>
       </c>
       <c r="B159" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>15083495650000</v>
+        <v>15073772090716</v>
       </c>
       <c r="B160" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C160" s="3"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>2009417000500</v>
+        <v>15075575690700</v>
       </c>
       <c r="B161" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C161" s="3"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>15031410580900</v>
+        <v>9096278380700</v>
       </c>
       <c r="B162" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C162" s="3"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>15052714680100</v>
+        <v>15052063990716</v>
       </c>
       <c r="B163" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>15589978940400</v>
+        <v>15021130970901</v>
       </c>
       <c r="B164" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C164" s="3"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>15010623600400</v>
+        <v>15049007600100</v>
       </c>
       <c r="B165" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>5520139230300</v>
+        <v>11092100780700</v>
       </c>
       <c r="B166" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C166" s="3"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>15031498540800</v>
+        <v>46590165350900</v>
       </c>
       <c r="B167" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>15086219020800</v>
+        <v>9595992810000</v>
       </c>
       <c r="B168" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C168" s="3"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>15031777950100</v>
+        <v>15043863830700</v>
       </c>
       <c r="B169" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>15026259520101</v>
+        <v>15049588570800</v>
       </c>
       <c r="B170" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C170" s="3"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>15585363400900</v>
+        <v>13055083660300</v>
       </c>
       <c r="B171" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C171" s="3"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>15044314040800</v>
+        <v>9561309640100</v>
       </c>
       <c r="B172" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C172" s="3"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>11521381000800</v>
+        <v>15011522410900</v>
       </c>
       <c r="B173" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C173" s="3"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>15533496881100</v>
+        <v>15587865340700</v>
       </c>
       <c r="B174" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C174" s="3"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>15060169930800</v>
+        <v>15524478320000</v>
       </c>
       <c r="B175" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C175" s="3"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>14594248470500</v>
+        <v>14592894090100</v>
       </c>
       <c r="B176" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C176" s="3"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>15084721410100</v>
+        <v>15021130970900</v>
       </c>
       <c r="B177" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C177" s="3"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>15023658490100</v>
+        <v>15043511480101</v>
       </c>
       <c r="B178" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C178" s="3"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>15088215870600</v>
+        <v>15032839340300</v>
       </c>
       <c r="B179" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>11095379790800</v>
+        <v>40507102310900</v>
       </c>
       <c r="B180" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C180" s="3"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>15078069070300</v>
+        <v>15583838450200</v>
       </c>
       <c r="B181" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>15014028790400</v>
+        <v>15031640950900</v>
       </c>
       <c r="B182" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C182" s="3"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>15081799660100</v>
+        <v>46590083030101</v>
       </c>
       <c r="B183" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>15013921260700</v>
+        <v>15087703520000</v>
       </c>
       <c r="B184" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C184" s="3"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>15053494560100</v>
+        <v>15024666350100</v>
       </c>
       <c r="B185" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C185" s="3"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>4010284340800</v>
+        <v>15087565370601</v>
       </c>
       <c r="B186" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C186" s="3"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>15582319441400</v>
+        <v>15029288650600</v>
       </c>
       <c r="B187" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C187" s="3"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>10561961530100</v>
+        <v>15013586900400</v>
       </c>
       <c r="B188" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C188" s="3"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>15042335970700</v>
+        <v>15010954070800</v>
       </c>
       <c r="B189" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C189" s="3"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>9005349230700</v>
+        <v>15086139760700</v>
       </c>
       <c r="B190" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C190" s="3"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>15055817710900</v>
+        <v>40507063710300</v>
       </c>
       <c r="B191" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C191" s="3"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>15035475360600</v>
+        <v>15033740760600</v>
       </c>
       <c r="B192" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C192" s="3"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>14005974260600</v>
+        <v>15081884470300</v>
       </c>
       <c r="B193" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C193" s="3"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>15026946730500</v>
+        <v>15016129830700</v>
       </c>
       <c r="B194" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C194" s="3"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>15049831850500</v>
+        <v>14003202900400</v>
       </c>
       <c r="B195" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>15538289400516</v>
+        <v>15502464020800</v>
       </c>
       <c r="B196" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C196" s="3"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>9095199060800</v>
+        <v>15001540450900</v>
       </c>
       <c r="B197" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C197" s="3"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>15083943090000</v>
+        <v>15018745920100</v>
       </c>
       <c r="B198" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C198" s="3"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>15049671820100</v>
+        <v>13053892670100</v>
       </c>
       <c r="B199" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>15022618100200</v>
+        <v>15016481250600</v>
       </c>
       <c r="B200" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C200" s="3"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>15511000450400</v>
+        <v>15058469550200</v>
       </c>
       <c r="B201" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C201" s="3"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>15027517780100</v>
+        <v>15055636130800</v>
       </c>
       <c r="B202" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C202" s="3"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>15022477800800</v>
+        <v>15075790980800</v>
       </c>
       <c r="B203" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C203" s="3"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>15598573230900</v>
+        <v>15083495650000</v>
       </c>
       <c r="B204" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C204" s="3"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>46590287290500</v>
+        <v>15040008750900</v>
       </c>
       <c r="B205" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C205" s="3"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>15041889460200</v>
+        <v>15080294300200</v>
       </c>
       <c r="B206" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C206" s="3"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>15060785890100</v>
+        <v>3010174510700</v>
       </c>
       <c r="B207" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C207" s="3"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>40507819150200</v>
+        <v>15052456860000</v>
       </c>
       <c r="B208" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C208" s="3"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>15083289150300</v>
+        <v>15046897230300</v>
       </c>
       <c r="B209" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C209" s="3"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>15059316650800</v>
+        <v>15005891920800</v>
       </c>
       <c r="B210" s="1">
         <v>10</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>15591456680400</v>
+        <v>15514107690200</v>
       </c>
       <c r="B211" s="1">
         <v>10</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>11095379790816</v>
+        <v>15083342130300</v>
       </c>
       <c r="B212" s="1">
         <v>10</v>
@@ -2300,25 +2300,25 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>15034520610600</v>
+        <v>15061489920800</v>
       </c>
       <c r="B213" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C213" s="3"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>40507307050200</v>
+        <v>15084722670100</v>
       </c>
       <c r="B214" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C214" s="3"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>15017590970500</v>
+        <v>15017703940700</v>
       </c>
       <c r="B215" s="1">
         <v>10</v>
@@ -2327,34 +2327,34 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>15037416330400</v>
+        <v>5590242650100</v>
       </c>
       <c r="B216" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C216" s="3"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>11593957100600</v>
+        <v>1003916420100</v>
       </c>
       <c r="B217" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C217" s="3"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>2009226280700</v>
+        <v>6530625961000</v>
       </c>
       <c r="B218" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C218" s="3"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>14090932480200</v>
+        <v>15562070450700</v>
       </c>
       <c r="B219" s="1">
         <v>10</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>15040437110100</v>
+        <v>15059439300100</v>
       </c>
       <c r="B220" s="1">
         <v>10</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>15001052930000</v>
+        <v>15044688780600</v>
       </c>
       <c r="B221" s="1">
         <v>10</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>15028393790100</v>
+        <v>15069947690600</v>
       </c>
       <c r="B222" s="1">
         <v>10</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>15068119460600</v>
+        <v>15024407010100</v>
       </c>
       <c r="B223" s="1">
         <v>10</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>15036796620700</v>
+        <v>15066195970400</v>
       </c>
       <c r="B224" s="1">
         <v>10</v>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>46501931990900</v>
+        <v>11095773750100</v>
       </c>
       <c r="B225" s="1">
         <v>10</v>
@@ -2417,43 +2417,43 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>15010091340000</v>
+        <v>15593192870100</v>
       </c>
       <c r="B226" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C226" s="3"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>15069072230800</v>
+        <v>15020240430000</v>
       </c>
       <c r="B227" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C227" s="3"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>15051655100600</v>
+        <v>15063518060000</v>
       </c>
       <c r="B228" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C228" s="3"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>15098559440500</v>
+        <v>15052066080000</v>
       </c>
       <c r="B229" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C229" s="3"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>9092909500300</v>
+        <v>15026439930800</v>
       </c>
       <c r="B230" s="1">
         <v>10</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>15060235740100</v>
+        <v>11594490290100</v>
       </c>
       <c r="B231" s="1">
         <v>10</v>
@@ -2471,156 +2471,468 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>15097318920100</v>
+        <v>15028095550301</v>
       </c>
       <c r="B232" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C232" s="3"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>15006088660400</v>
+        <v>13050565610600</v>
       </c>
       <c r="B233" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C233" s="3"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>15018084590100</v>
+        <v>15086309000600</v>
       </c>
       <c r="B234" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C234" s="3"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>15017202370100</v>
+        <v>9595992810000</v>
       </c>
       <c r="B235" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C235" s="3"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>15031832480300</v>
+        <v>11521862820200</v>
       </c>
       <c r="B236" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C236" s="3"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>14091900940100</v>
+        <v>15063582620400</v>
       </c>
       <c r="B237" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C237" s="3"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>15030778850700</v>
+        <v>15052546570500</v>
       </c>
       <c r="B238" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C238" s="3"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>15528063040005</v>
+        <v>10053979200700</v>
       </c>
       <c r="B239" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C239" s="3"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>15027046450100</v>
+        <v>15069308400100</v>
       </c>
       <c r="B240" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C240" s="3"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>15076855530300</v>
+        <v>15035201650400</v>
       </c>
       <c r="B241" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C241" s="3"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>15040832450500</v>
+        <v>15006029040400</v>
       </c>
       <c r="B242" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C242" s="3"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>11595020050200</v>
+        <v>15010057240700</v>
       </c>
       <c r="B243" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C243" s="3"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>46590310310300</v>
+        <v>15089250550100</v>
       </c>
       <c r="B244" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C244" s="3"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>15057792390500</v>
+        <v>15535894290100</v>
       </c>
       <c r="B245" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C245" s="3"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>15023912910700</v>
+        <v>15003177820000</v>
       </c>
       <c r="B246" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C246" s="3"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>15035746200100</v>
+        <v>15043777240100</v>
       </c>
       <c r="B247" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C247" s="3"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>15584685550000</v>
+        <v>15055090080800</v>
       </c>
       <c r="B248" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C248" s="3"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>15027155420100</v>
+      </c>
+      <c r="B249" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>14594615540600</v>
+      </c>
+      <c r="B250" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>11091149880700</v>
+      </c>
+      <c r="B251" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>15018600250900</v>
+      </c>
+      <c r="B252" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>15022849340100</v>
+      </c>
+      <c r="B253" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>15018782803700</v>
+      </c>
+      <c r="B254" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>15030078450600</v>
+      </c>
+      <c r="B255" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>15070304860200</v>
+      </c>
+      <c r="B256" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>15030406830900</v>
+      </c>
+      <c r="B257" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>15022740940600</v>
+      </c>
+      <c r="B258" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>15034950550300</v>
+      </c>
+      <c r="B259" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>9596253390100</v>
+      </c>
+      <c r="B260" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>15586845150600</v>
+      </c>
+      <c r="B261" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>15085169930800</v>
+      </c>
+      <c r="B262" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>15040053820400</v>
+      </c>
+      <c r="B263" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>15074410060100</v>
+      </c>
+      <c r="B264" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>15020347980000</v>
+      </c>
+      <c r="B265" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>15086361560700</v>
+      </c>
+      <c r="B266" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>14001795280300</v>
+      </c>
+      <c r="B267" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>1010251820100</v>
+      </c>
+      <c r="B268" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>15058732970000</v>
+      </c>
+      <c r="B269" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>15040437110100</v>
+      </c>
+      <c r="B270" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>15057611890000</v>
+      </c>
+      <c r="B271" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>15044314820300</v>
+      </c>
+      <c r="B272" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>15014825880700</v>
+      </c>
+      <c r="B273" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>15026189130416</v>
+      </c>
+      <c r="B274" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>15017272630300</v>
+      </c>
+      <c r="B275" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>15006083830900</v>
+      </c>
+      <c r="B276" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>15067020220600</v>
+      </c>
+      <c r="B277" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>15025007590600</v>
+      </c>
+      <c r="B278" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>15024320220800</v>
+      </c>
+      <c r="B279" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>15082938190900</v>
+      </c>
+      <c r="B280" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>13054660450200</v>
+      </c>
+      <c r="B281" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>15064962520300</v>
+      </c>
+      <c r="B282" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>15030076580600</v>
+      </c>
+      <c r="B283" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>15028533540100</v>
+      </c>
+      <c r="B284" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>11094589220400</v>
+      </c>
+      <c r="B285" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
+        <v>10052737380000</v>
+      </c>
+      <c r="B286" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>15040974450100</v>
+      </c>
+      <c r="B287" s="1">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>